<commit_message>
fixed template rendering issues
</commit_message>
<xml_diff>
--- a/static/data/categories_complete.xlsx
+++ b/static/data/categories_complete.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web_proyects\imprenta_gallito\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC933E6D-B54E-4AED-AFE9-DD779FE002B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099CD67C-A7C4-48CF-8E74-E4B4368B4456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900"/>
+    <workbookView xWindow="20" yWindow="200" windowWidth="34380" windowHeight="13570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categories_complete" sheetId="1" r:id="rId1"/>
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1060,12 +1060,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
antes de agregar sexo en el registro
</commit_message>
<xml_diff>
--- a/static/data/categories_complete.xlsx
+++ b/static/data/categories_complete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web_proyects\imprenta_gallito\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099CD67C-A7C4-48CF-8E74-E4B4368B4456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EF800C-BFD4-4058-B6C9-9D6F82E7D956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="200" windowWidth="34380" windowHeight="13570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="110" windowWidth="34380" windowHeight="13570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categories_complete" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>category_slug</t>
   </si>
@@ -152,63 +152,6 @@
   </si>
   <si>
     <t>occasions</t>
-  </si>
-  <si>
-    <t>logo-web-social</t>
-  </si>
-  <si>
-    <t>Logo Sitios Web y Redes Sociales</t>
-  </si>
-  <si>
-    <t>Diseño de identidad corporativa y presencia digital</t>
-  </si>
-  <si>
-    <t>/media/category_images/redes_sociales.jpg</t>
-  </si>
-  <si>
-    <t>services</t>
-  </si>
-  <si>
-    <t>servicios-diseno</t>
-  </si>
-  <si>
-    <t>Servicios de Diseño</t>
-  </si>
-  <si>
-    <t>Servicios profesionales de diseño gráfico</t>
-  </si>
-  <si>
-    <t>/media/category_images/servicios_diseno.jpg</t>
-  </si>
-  <si>
-    <t>black-friday</t>
-  </si>
-  <si>
-    <t>Venta de Black Friday</t>
-  </si>
-  <si>
-    <t>Ofertas y descuentos especiales durante Black Friday</t>
-  </si>
-  <si>
-    <t>/media/category_images/black_friday.jpg</t>
-  </si>
-  <si>
-    <t>seasonal</t>
-  </si>
-  <si>
-    <t>standard</t>
-  </si>
-  <si>
-    <t>tarjetas-navidad</t>
-  </si>
-  <si>
-    <t>Tarjetas de Navidad y Festividades</t>
-  </si>
-  <si>
-    <t>Tarjetas personalizadas para Navidad y celebraciones</t>
-  </si>
-  <si>
-    <t>/media/category_images/navidad.jpg</t>
   </si>
   <si>
     <t>calendarios-regalos</t>
@@ -1061,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1293,104 +1236,12 @@
         <v>47</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>